<commit_message>
this branch is terminated
</commit_message>
<xml_diff>
--- a/logFile-analysis 28052016.2016.xlsx
+++ b/logFile-analysis 28052016.2016.xlsx
@@ -1499,15 +1499,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>828674</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>866774</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>666749</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1830,7 +1830,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D33"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,10 +1880,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>3</v>
       </c>
       <c r="C2">
@@ -1929,10 +1929,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>5</v>
       </c>
       <c r="C3">
@@ -3000,8 +3000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C360"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159:C239"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>